<commit_message>
Creating LdIndexManager class to manage all indexes
</commit_message>
<xml_diff>
--- a/src/test/resources/ws353simrel/wordsim_DBpedia.xlsx
+++ b/src/test/resources/ws353simrel/wordsim_DBpedia.xlsx
@@ -1107,7 +1107,7 @@
   <dimension ref="A1:O65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1296,8 +1296,8 @@
       <c r="L4">
         <v>6.3334039999999994E-2</v>
       </c>
-      <c r="M4" s="1">
-        <v>-1.3699999999999999E-5</v>
+      <c r="M4">
+        <v>0</v>
       </c>
       <c r="N4" t="s">
         <v>13</v>
@@ -1343,8 +1343,8 @@
       <c r="L5">
         <v>2.1221355000000001E-2</v>
       </c>
-      <c r="M5" s="1">
-        <v>-1.06E-5</v>
+      <c r="M5">
+        <v>0</v>
       </c>
       <c r="N5" t="s">
         <v>13</v>
@@ -1437,8 +1437,8 @@
       <c r="L7">
         <v>6.7087158999999993E-2</v>
       </c>
-      <c r="M7" s="1">
-        <v>-2.8600000000000001E-5</v>
+      <c r="M7">
+        <v>0</v>
       </c>
       <c r="N7" t="s">
         <v>13</v>

</xml_diff>